<commit_message>
easier create recipe interface
</commit_message>
<xml_diff>
--- a/trackers/2025-12.xlsx
+++ b/trackers/2025-12.xlsx
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1344,7 +1344,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -1352,7 +1352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1915,7 +1915,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -1923,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2614,7 +2614,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -2622,7 +2622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3345,7 +3345,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -3353,7 +3353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -4012,7 +4012,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -4020,7 +4020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -4615,7 +4615,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -4623,7 +4623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -5058,6 +5058,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>